<commit_message>
Adding metal domes to bom.
</commit_message>
<xml_diff>
--- a/remote eagle/turntouch-remote-master-bom.xlsx
+++ b/remote eagle/turntouch-remote-master-bom.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="65">
   <si>
     <t>TURNTUCH REMOTE MASTER</t>
   </si>
@@ -70,7 +70,7 @@
     <t>www.raytac.com</t>
   </si>
   <si>
-    <t>nRF51422 BLE SoC module with chip antenna</t>
+    <t>nRF51422 BLE SoC module with PCB trace antenna</t>
   </si>
   <si>
     <t>SMD module</t>
@@ -192,6 +192,32 @@
   </si>
   <si>
     <t>HOLDER BATTERY 20MM COIN</t>
+  </si>
+  <si>
+    <t>TS1; TS2; TS3; TS4</t>
+  </si>
+  <si>
+    <t>CMD</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>www.china-metaldome.com</t>
+    </r>
+  </si>
+  <si>
+    <t>Metal dome sticker array backed with adhesive tape</t>
+  </si>
+  <si>
+    <t>Bulk</t>
+  </si>
+  <si>
+    <t>Sticker array</t>
   </si>
   <si>
     <t>TOTAL SUM</t>
@@ -205,7 +231,7 @@
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="59" formatCode="&quot;$&quot;0.00"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -217,6 +243,12 @@
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color indexed="12"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u val="single"/>
       <sz val="10"/>
       <color indexed="12"/>
       <name val="Arial"/>
@@ -394,7 +426,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -472,6 +504,12 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="59" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
@@ -644,13 +682,7 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -740,19 +772,19 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1007,13 +1039,7 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
+        <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -1317,19 +1343,19 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1754,7 +1780,7 @@
         <v>5</v>
       </c>
       <c r="M7" s="18">
-        <v>5</v>
+        <v>3.55</v>
       </c>
     </row>
     <row r="8" ht="14.9" customHeight="1">
@@ -2166,19 +2192,39 @@
       </c>
     </row>
     <row r="18" ht="12.8" customHeight="1">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
+      <c r="A18" s="26">
+        <v>12</v>
+      </c>
+      <c r="B18" t="s" s="20">
+        <v>58</v>
+      </c>
+      <c r="C18" s="26">
+        <v>1</v>
+      </c>
       <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
+      <c r="E18" t="s" s="20">
+        <v>59</v>
+      </c>
       <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
+      <c r="G18" t="s" s="20">
+        <v>60</v>
+      </c>
       <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="26"/>
-      <c r="M18" s="26"/>
+      <c r="I18" t="s" s="20">
+        <v>61</v>
+      </c>
+      <c r="J18" t="s" s="20">
+        <v>62</v>
+      </c>
+      <c r="K18" t="s" s="27">
+        <v>63</v>
+      </c>
+      <c r="L18" s="28">
+        <v>2</v>
+      </c>
+      <c r="M18" s="28">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="19" ht="12.8" customHeight="1">
       <c r="A19" s="5"/>
@@ -2191,16 +2237,16 @@
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="2"/>
-      <c r="K19" t="s" s="27">
-        <v>58</v>
-      </c>
-      <c r="L19" s="28">
-        <f>SUM(L7:L17)</f>
-        <v>6.879999999999997</v>
-      </c>
-      <c r="M19" s="29">
-        <f>SUM(M7:M17)</f>
-        <v>5.879380000000003</v>
+      <c r="K19" t="s" s="29">
+        <v>64</v>
+      </c>
+      <c r="L19" s="30">
+        <f>SUM(L7:L18)</f>
+        <v>8.879999999999997</v>
+      </c>
+      <c r="M19" s="31">
+        <f>SUM(M7:M18)</f>
+        <v>4.679380000000003</v>
       </c>
     </row>
   </sheetData>
@@ -2219,6 +2265,7 @@
     <hyperlink ref="G15" r:id="rId8" location="" tooltip="" display=""/>
     <hyperlink ref="G16" r:id="rId9" location="" tooltip="" display=""/>
     <hyperlink ref="G17" r:id="rId10" location="" tooltip="" display=""/>
+    <hyperlink ref="G18" r:id="rId11" location="" tooltip="" display=""/>
   </hyperlinks>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="landscape" pageOrder="downThenOver"/>

</xml_diff>